<commit_message>
Patched augmentation notebook to load imports and use rdfs labels as last resort for definitions.
</commit_message>
<xml_diff>
--- a/projects/project-3/assignment/src/data/ccom-qudt-structural-matches-with-defs.xlsx
+++ b/projects/project-3/assignment/src/data/ccom-qudt-structural-matches-with-defs.xlsx
@@ -526,8 +526,16 @@
           <t>SubClassOf: qudt-v1:PhysicalUnit | SubClassOf: qudt-v1:typePrefix value UAP</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Atomic Physics Unit</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -570,8 +578,16 @@
           <t>SubClassOf: qudt-v1:ScienceAndEngineeringUnit | SubClassOf: qudt-v1:typePrefix value UPHS</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Physical Unit</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -614,8 +630,16 @@
           <t>SubClassOf: qudt-v1:Unit | SubClassOf: qudt-v1:typePrefix value USE</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Science And Engineering Unit</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -658,8 +682,16 @@
           <t>SubClassOf: qudt-v1:PhysicalUnit | SubClassOf: qudt-v1:typePrefix value UCHM</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Chemistry Unit</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -702,8 +734,16 @@
           <t>SubClassOf: qudt-v1:PhysicalUnit | SubClassOf: qudt-v1:typePrefix value UTD</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Thermodynamics Unit</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -746,8 +786,16 @@
           <t>SubClassOf: qudt-v1:PhysicalUnit | SubClassOf: qudt-v1:typePrefix value UMH</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Mechanics Unit</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -790,8 +838,16 @@
           <t>SubClassOf: qudt-v1:PhysicalUnit | SubClassOf: qudt-v1:typePrefix value UROY</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Radiology Unit</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -834,8 +890,16 @@
           <t>SubClassOf: qudt-v1:ScienceAndEngineeringUnit | SubClassOf: qudt-v1:typePrefix value UBM</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Biomedical Unit</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -878,8 +942,16 @@
           <t>SubClassOf: qudt-v1:ScienceAndEngineeringUnit | SubClassOf: qudt-v1:typePrefix value UCMN</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Communications Unit</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -922,8 +994,16 @@
           <t>SubClassOf: qudt-v1:PhysicalUnit | SubClassOf: qudt-v1:typePrefix value UEM</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Electricity And Magnetism Unit</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -966,8 +1046,16 @@
           <t>SubClassOf: qudt-v1:PhysicalUnit | SubClassOf: qudt-v1:typePrefix value UST</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Space And Time Unit</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1010,8 +1098,16 @@
           <t>SubClassOf: qudt-v1:FinancialUnit | SubClassOf: qudt-v1:currencyExponent exactly 1 | SubClassOf: qudt-v1:typePrefix value UFC</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Currency Unit</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1054,8 +1150,16 @@
           <t>SubClassOf: qudt-v1:ResourceUnit | SubClassOf: qudt-v1:typePrefix value UH</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Human Unit</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1098,8 +1202,16 @@
           <t>SubClassOf: qudt-v1:ResourceUnit | SubClassOf: qudt-v1:typePrefix value UF</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Financial Unit</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1142,8 +1254,16 @@
           <t>SubClassOf: qudt-v1:ScienceAndEngineeringUnit | SubClassOf: qudt-v1:typePrefix value UCPG</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr"/>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>An Information Content Entity that consists of a set of propositions that describe some Entity.</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Computing Unit</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>